<commit_message>
ducanh 30/11 ver3 Signed-off-by:Leanhduc09112004 <cooperanh092004@gmail.com>
</commit_message>
<xml_diff>
--- a/DanhSachNhanVien.xlsx
+++ b/DanhSachNhanVien.xlsx
@@ -68,7 +68,7 @@
     <t>Hà Nội</t>
   </si>
   <si>
-    <t>cooperanh092004@gmail.com</t>
+    <t>anhldph44493@fpt.edu.vn</t>
   </si>
   <si>
     <t>Quản lí</t>
@@ -77,7 +77,7 @@
     <t>Đang làm</t>
   </si>
   <si>
-    <t>09112004</t>
+    <t>09112004le</t>
   </si>
   <si>
     <t>NV002</t>

</xml_diff>